<commit_message>
additional pairwis post hoc for 2019 models
</commit_message>
<xml_diff>
--- a/evenness_metric.xlsx
+++ b/evenness_metric.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kailigregory/Desktop/Cornell/Thesis/GitHub/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30DAB180-1381-3742-BF3A-4C4B81CEE56A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83404AB7-91C4-724D-B59F-DD14EF24A66B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1760" yWindow="500" windowWidth="26740" windowHeight="16020" xr2:uid="{55E1E4E0-7A1F-D546-BD82-805FD7AA8EA0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="20940" windowHeight="16160" xr2:uid="{55E1E4E0-7A1F-D546-BD82-805FD7AA8EA0}"/>
   </bookViews>
   <sheets>
-    <sheet name="evenness" sheetId="4" r:id="rId1"/>
+    <sheet name="indices" sheetId="4" r:id="rId1"/>
     <sheet name="wild" sheetId="1" r:id="rId2"/>
     <sheet name="hatchery" sheetId="3" r:id="rId3"/>
     <sheet name="aq" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -219,22 +219,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>774013</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:colOff>533399</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>193673</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>770000</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>79375</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="Chart&#10;&#10;Description automatically generated">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0116923F-1B9A-AC42-AC06-62EDF14769AF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4D0C4AD-01E9-A149-9E97-D8FF07818140}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -243,21 +243,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4901513" y="1028700"/>
-          <a:ext cx="10401987" cy="7213600"/>
+          <a:off x="4660899" y="400048"/>
+          <a:ext cx="10968101" cy="7727952"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -269,15 +263,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
+      <xdr:colOff>288925</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:rowOff>41275</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -292,8 +286,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6654800" y="1562100"/>
-          <a:ext cx="1193800" cy="1930400"/>
+          <a:off x="6892925" y="1485900"/>
+          <a:ext cx="1193800" cy="1958975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -346,9 +340,6 @@
           <a:endParaRPr lang="en-US" sz="1300" baseline="0"/>
         </a:p>
         <a:p>
-          <a:endParaRPr lang="en-US" sz="1300" baseline="0"/>
-        </a:p>
-        <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1300" baseline="0"/>
             <a:t>0.42 ; 0.69</a:t>
@@ -361,15 +352,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>22225</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>587375</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -384,8 +375,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6680200" y="3416300"/>
-          <a:ext cx="1193800" cy="1612900"/>
+          <a:off x="6823075" y="3117850"/>
+          <a:ext cx="1193800" cy="1638300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -456,15 +447,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>98425</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -479,8 +470,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6604000" y="5257800"/>
-          <a:ext cx="1193800" cy="1612900"/>
+          <a:off x="6858000" y="4845050"/>
+          <a:ext cx="1193800" cy="1638300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -547,16 +538,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>812113</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>129488</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>196850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>354913</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:colOff>497788</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -571,8 +562,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9892613" y="1524000"/>
-          <a:ext cx="1193800" cy="1612900"/>
+          <a:off x="10035488" y="1435100"/>
+          <a:ext cx="1193800" cy="1638300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -627,16 +618,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>748613</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>65988</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>291413</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:colOff>434288</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -651,8 +642,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9829113" y="3403600"/>
-          <a:ext cx="1193800" cy="1612900"/>
+          <a:off x="9971988" y="3121025"/>
+          <a:ext cx="1193800" cy="1638300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -719,16 +710,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>786713</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>56463</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>329513</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:colOff>424763</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -743,8 +734,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9867213" y="5257800"/>
-          <a:ext cx="1193800" cy="1612900"/>
+          <a:off x="9962463" y="4829175"/>
+          <a:ext cx="1193800" cy="1638300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -812,15 +803,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>596213</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:colOff>659713</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>155575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>139013</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:colOff>202513</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -835,8 +826,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12978713" y="1562100"/>
-          <a:ext cx="1193800" cy="1612900"/>
+          <a:off x="13042213" y="1393825"/>
+          <a:ext cx="1193800" cy="1638300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -907,15 +898,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>608913</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>735913</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>41275</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>151713</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:colOff>278713</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -930,8 +921,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12991413" y="3403600"/>
-          <a:ext cx="1193800" cy="1612900"/>
+          <a:off x="13118413" y="3136900"/>
+          <a:ext cx="1193800" cy="1638300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1002,15 +993,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>672413</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:colOff>751788</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>215213</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:colOff>294588</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1025,8 +1016,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13054913" y="5270500"/>
-          <a:ext cx="1193800" cy="1612900"/>
+          <a:off x="13134288" y="4873625"/>
+          <a:ext cx="1193800" cy="1638300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1396,8 +1387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93716CDA-E8BB-9647-94A4-ECD954C3524F}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U21" sqref="U21"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3633,7 +3624,7 @@
         <v>18</v>
       </c>
       <c r="F2">
-        <f t="shared" ref="F2:F62" si="0">LN(B2)</f>
+        <f t="shared" ref="F2:F61" si="0">LN(B2)</f>
         <v>-1.4663370677934271</v>
       </c>
       <c r="G2">
@@ -5312,7 +5303,7 @@
         <v>19</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F2:F61" si="0">LN(B3)</f>
+        <f t="shared" ref="F3:F61" si="0">LN(B3)</f>
         <v>-0.77318988723348181</v>
       </c>
       <c r="G3">

</xml_diff>